<commit_message>
tidy up data pipeline
</commit_message>
<xml_diff>
--- a/Results/Codes and classifications/IPCC_regions.xlsx
+++ b/Results/Codes and classifications/IPCC_regions.xlsx
@@ -20,7 +20,7 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">region_ar6_5</t>
+    <t xml:space="preserve">region_ar6_6</t>
   </si>
   <si>
     <t xml:space="preserve">region_ar6_10</t>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">region_ar6_dev</t>
   </si>
   <si>
-    <t xml:space="preserve">region_ar6_5_short</t>
+    <t xml:space="preserve">region_ar6_6_short</t>
   </si>
   <si>
     <t xml:space="preserve">AFG</t>

</xml_diff>